<commit_message>
Stabalized the amplifier code
</commit_message>
<xml_diff>
--- a/master_nodes.xlsx
+++ b/master_nodes.xlsx
@@ -9,14 +9,15 @@
   <sheets>
     <sheet name="Nodes" sheetId="1" r:id="rId1"/>
     <sheet name="Nodes_metadata" sheetId="2" r:id="rId2"/>
-    <sheet name="Nodes_metadata_start" sheetId="3" r:id="rId3"/>
+    <sheet name="Nodes_amplifiers" sheetId="3" r:id="rId3"/>
+    <sheet name="Nodes_metadata_start" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
   <si>
     <t>FROM</t>
   </si>
@@ -39,13 +40,25 @@
     <t>LINK ID</t>
   </si>
   <si>
-    <t>Distance</t>
-  </si>
-  <si>
-    <t>AMPLIFIERS NODES</t>
-  </si>
-  <si>
-    <t>AMPLIFIERS TYPE</t>
+    <t>DISTANCE</t>
+  </si>
+  <si>
+    <t>AMPLIFIERS</t>
+  </si>
+  <si>
+    <t>AMPLIFIER FROM</t>
+  </si>
+  <si>
+    <t>AMPLIFIER TO</t>
+  </si>
+  <si>
+    <t>AMPLIFIER TYPE</t>
+  </si>
+  <si>
+    <t>AMPLIFIER ID</t>
+  </si>
+  <si>
+    <t>AMPLIFIER DISTANCE</t>
   </si>
   <si>
     <t>Hyderabad</t>
@@ -60,6 +73,9 @@
     <t>None</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>Mumbai</t>
   </si>
   <si>
@@ -93,89 +109,110 @@
     <t>L</t>
   </si>
   <si>
-    <t>Ramanagara, Madduru</t>
-  </si>
-  <si>
-    <t>A, B</t>
+    <t>Ramanagara</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Mandya</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
   <si>
     <t>FROM_EDITED</t>
   </si>
   <si>
+    <t>FROM_COORDINATES</t>
+  </si>
+  <si>
     <t>TO_EDITED</t>
   </si>
   <si>
-    <t>FROM_COORDINATES</t>
-  </si>
-  <si>
     <t>TO_COORDINATES</t>
   </si>
   <si>
     <t>Hyderabad, India</t>
   </si>
   <si>
+    <t>17.41500345,78.4193658848225</t>
+  </si>
+  <si>
     <t>Vishakapatnam, India</t>
   </si>
   <si>
-    <t>17.41500345,78.4193658848225</t>
-  </si>
-  <si>
     <t>17.72131135,83.2900511199386</t>
   </si>
   <si>
     <t>Mumbai, India</t>
   </si>
   <si>
+    <t>18.9321862,72.8308337</t>
+  </si>
+  <si>
     <t>Pune, India</t>
   </si>
   <si>
-    <t>18.9321862,72.8308337</t>
-  </si>
-  <si>
     <t>18.5203062,73.8543185</t>
   </si>
   <si>
     <t>Chennai, India</t>
   </si>
   <si>
+    <t>13.0801721,80.2838331</t>
+  </si>
+  <si>
     <t>Thanjavur, India</t>
   </si>
   <si>
-    <t>13.0801721,80.2838331</t>
-  </si>
-  <si>
     <t>10.7860689,79.1381282</t>
   </si>
   <si>
     <t>Kochi, India</t>
   </si>
   <si>
+    <t>9.9633864,76.2536614</t>
+  </si>
+  <si>
     <t>Coimbatore, India</t>
   </si>
   <si>
-    <t>9.9633864,76.2536614</t>
-  </si>
-  <si>
     <t>11.0018115,76.9628425</t>
   </si>
   <si>
-    <t>Bengaluru, India</t>
-  </si>
-  <si>
-    <t>Mysuru, India</t>
+    <t>Bengaluru ,India</t>
   </si>
   <si>
     <t>12.9791198,77.5912997</t>
   </si>
   <si>
+    <t>Ramanagara ,India</t>
+  </si>
+  <si>
+    <t>12.7252766,77.2804797</t>
+  </si>
+  <si>
+    <t>Mandya ,India</t>
+  </si>
+  <si>
+    <t>12.5238888,76.8961961</t>
+  </si>
+  <si>
+    <t>Mysuru ,India</t>
+  </si>
+  <si>
     <t>12.3051828,76.6553609</t>
+  </si>
+  <si>
+    <t>AMPLIFIER_FROM_COORDINATES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,10 +223,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -215,7 +256,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -283,25 +324,84 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,327 +696,502 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.28515625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="2" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2">
+      <c r="M1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2">
+      <c r="H2" s="5">
         <v>100</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1">
         <v>13</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="2" t="s">
+      <c r="H3" s="5">
+        <v>200</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1">
         <v>14</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="H4" s="5">
+        <v>300</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1">
         <v>15</v>
       </c>
-      <c r="C3" s="2">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="2">
-        <v>13</v>
-      </c>
-      <c r="H3" s="2">
-        <v>200</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="2" t="s">
+      <c r="H5" s="5">
+        <v>400</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="2">
-        <v>14</v>
-      </c>
-      <c r="H4" s="2">
-        <v>300</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="2" t="s">
+      <c r="J5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1</v>
+      </c>
+      <c r="D6" s="12">
+        <v>6</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="12">
+        <v>11</v>
+      </c>
+      <c r="H6" s="12">
+        <v>500</v>
+      </c>
+      <c r="I6" s="12">
+        <v>2</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="9">
         <v>20</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="N6" s="9">
+        <v>48.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="9">
         <v>21</v>
       </c>
-      <c r="C5" s="2">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="2">
-        <v>15</v>
-      </c>
-      <c r="H5" s="2">
-        <v>400</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2">
-        <v>6</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="2">
-        <v>11</v>
-      </c>
-      <c r="H6" s="2">
-        <v>500</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>26</v>
+      <c r="N7" s="9">
+        <v>52.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="9">
+        <v>46.2</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="H6:H8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="30.28515625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="3"/>
-      <c r="B1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>30</v>
+      <c r="A1" s="2"/>
+      <c r="B1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="5">
+      <c r="A2" s="11">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="5">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="5">
+      <c r="A4" s="11">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="5">
+      <c r="A5" s="11">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="5">
+      <c r="A6" s="11">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="11">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -925,6 +1200,92 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="14.42578125" style="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="6"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="6"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="6"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="6"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="6"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="6"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
@@ -934,17 +1295,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>28</v>
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added support to plot source and destination for links containing amplifiers
</commit_message>
<xml_diff>
--- a/master_nodes.xlsx
+++ b/master_nodes.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="1"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Nodes" sheetId="1" r:id="rId1"/>
-    <sheet name="Nodes_metadata" sheetId="2" r:id="rId2"/>
-    <sheet name="Nodes_amplifiers" sheetId="3" r:id="rId3"/>
-    <sheet name="Nodes_metadata_start" sheetId="4" r:id="rId4"/>
+    <sheet name="Nodes" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Nodes_metadata" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Nodes_amplifiers" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Nodes_metadata_start" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
   <si>
     <t>FROM</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Coimbatore</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
   <si>
     <t>Bengaluru</t>
@@ -212,51 +215,55 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <numFmts count="0"/>
+  <fonts count="7">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -367,47 +374,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="17">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="7" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="1" borderId="9" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -695,22 +726,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="7" max="7" width="18.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="18.28515625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="13" width="18.28515625"/>
+    <col customWidth="1" max="9" min="8" style="13" width="18.28515625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="13" width="16.28515625"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="13" width="12.7109375"/>
+    <col bestFit="1" customWidth="1" max="12" min="12" style="13" width="19.85546875"/>
+    <col bestFit="1" customWidth="1" max="13" min="13" style="13" width="12.7109375"/>
+    <col bestFit="1" customWidth="1" max="14" min="14" style="13" width="19.85546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -764,10 +799,10 @@
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1" t="n">
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -776,10 +811,10 @@
       <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="5" t="n">
         <v>100</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -808,10 +843,10 @@
       <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="1" t="n">
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -820,10 +855,10 @@
       <c r="F3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="5" t="n">
         <v>200</v>
       </c>
       <c r="I3" s="5" t="s">
@@ -852,10 +887,10 @@
       <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="n">
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -864,10 +899,10 @@
       <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="5" t="n">
         <v>300</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -896,22 +931,22 @@
       <c r="B5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1">
+        <v>27</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="5" t="n">
         <v>400</v>
       </c>
       <c r="I5" s="5" t="s">
@@ -935,97 +970,79 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="12">
+      <c r="B6" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="12" t="n">
         <v>6</v>
       </c>
       <c r="E6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="H6" s="12" t="n">
+        <v>500</v>
+      </c>
+      <c r="I6" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="9" t="n">
+        <v>20</v>
+      </c>
+      <c r="N6" s="9" t="n">
+        <v>48.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="J7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="9" t="n">
+        <v>21</v>
+      </c>
+      <c r="N7" s="9" t="n">
+        <v>52.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="J8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="12">
-        <v>11</v>
-      </c>
-      <c r="H6" s="12">
-        <v>500</v>
-      </c>
-      <c r="I6" s="12">
-        <v>2</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" s="9">
-        <v>20</v>
-      </c>
-      <c r="N6" s="9">
-        <v>48.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" s="9">
-        <v>21</v>
-      </c>
-      <c r="N7" s="9">
-        <v>52.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="L8" s="4" t="s">
         <v>18</v>
       </c>
       <c r="M8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N8" s="9" t="n">
         <v>46.2</v>
       </c>
     </row>
@@ -1041,175 +1058,183 @@
     <mergeCell ref="D6:D8"/>
     <mergeCell ref="H6:H8"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="30.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="13" width="17.42578125"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="13" width="28.28515625"/>
+    <col bestFit="1" customWidth="1" max="5" min="4" style="13" width="30.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="2"/>
-      <c r="B1" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="11" t="s">
+      <c r="A1" s="2" t="n"/>
+      <c r="B1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="D1" s="16" t="s">
         <v>37</v>
       </c>
+      <c r="E1" s="16" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="11">
+      <c r="A2" s="16" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="11">
+      <c r="A3" s="16" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="11">
+      <c r="A4" s="16" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="11">
+      <c r="A5" s="16" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="11">
+      <c r="A6" s="16" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="11">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="11">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>58</v>
-      </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="4" max="4" width="14.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="13" width="14.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -1256,59 +1281,63 @@
         <v>13</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="6"/>
+      <c r="A2" s="6" t="n"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="6"/>
+      <c r="A3" s="6" t="n"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="6"/>
+      <c r="A4" s="6" t="n"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="6"/>
+      <c r="A5" s="6" t="n"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="6"/>
+      <c r="A6" s="6" t="n"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="6"/>
+      <c r="A7" s="6" t="n"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="6"/>
+      <c r="A8" s="6" t="n"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="13" width="13.7109375"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="13" width="10.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2"/>
+      <c r="A1" s="2" t="n"/>
       <c r="B1" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added support o ignore .xlsx files
</commit_message>
<xml_diff>
--- a/master_nodes.xlsx
+++ b/master_nodes.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="1"/>
+    <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Nodes" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Nodes_metadata" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Nodes_metadata_start" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Nodes" sheetId="1" r:id="rId1"/>
+    <sheet name="Nodes_metadata" sheetId="2" r:id="rId2"/>
+    <sheet name="Nodes_metadata_start" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
   <si>
     <t>FROM</t>
   </si>
@@ -211,59 +211,41 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-  </numFmts>
-  <fonts count="7">
+  <fonts count="4">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Cambria"/>
-      <charset val="1"/>
-      <family val="1"/>
-      <b val="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -272,76 +254,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" name="Comma" xfId="1"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="5" name="Percent" xfId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -629,30 +628,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:N8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AMK8"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B6" activeCellId="0" pane="topLeft" sqref="B6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="6" min="1" style="8" width="8.5748987854251"/>
-    <col customWidth="1" max="9" min="7" style="8" width="18.2834008097166"/>
-    <col customWidth="1" max="10" min="10" style="8" width="16.2834008097166"/>
-    <col customWidth="1" max="11" min="11" style="8" width="12.7125506072875"/>
-    <col customWidth="1" max="12" min="12" style="8" width="19.8542510121458"/>
-    <col customWidth="1" max="13" min="13" style="8" width="12.7125506072875"/>
-    <col customWidth="1" max="14" min="14" style="8" width="19.8542510121458"/>
-    <col customWidth="1" max="1025" min="15" style="8" width="8.5748987854251"/>
+    <col min="1" max="6" width="8.5703125" style="6" customWidth="1"/>
+    <col min="7" max="9" width="18.28515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" style="6" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="6" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" style="6" customWidth="1"/>
+    <col min="15" max="1025" width="8.5703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="8" spans="1:14">
+    <row r="1" spans="1:14" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -696,17 +691,17 @@
         <v>13</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" s="8" spans="1:14">
+    <row r="2" spans="1:14" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="2">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="2">
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -715,10 +710,10 @@
       <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="2">
         <v>12</v>
       </c>
-      <c r="H2" s="3" t="n">
+      <c r="H2" s="3">
         <v>100</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -740,17 +735,17 @@
         <v>18</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3" s="8" spans="1:14">
+    <row r="3" spans="1:14" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="2">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="2">
         <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -759,10 +754,10 @@
       <c r="F3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="2">
         <v>13</v>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" s="3">
         <v>200</v>
       </c>
       <c r="I3" s="3" t="s">
@@ -784,17 +779,17 @@
         <v>18</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="4" s="8" spans="1:14">
+    <row r="4" spans="1:14" ht="15" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="2">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="2">
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -803,10 +798,10 @@
       <c r="F4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="2">
         <v>14</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="3">
         <v>300</v>
       </c>
       <c r="I4" s="3" t="s">
@@ -828,17 +823,17 @@
         <v>18</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="5" s="8" spans="1:14">
+    <row r="5" spans="1:14" ht="15" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="2">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="2">
         <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -847,10 +842,10 @@
       <c r="F5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="2">
         <v>15</v>
       </c>
-      <c r="H5" s="3" t="n">
+      <c r="H5" s="3">
         <v>400</v>
       </c>
       <c r="I5" s="3" t="s">
@@ -872,32 +867,32 @@
         <v>18</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="6" s="8" spans="1:14">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:14" ht="15" customHeight="1">
+      <c r="A6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="C6" s="8">
         <v>1</v>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D6" s="8">
         <v>6</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="8">
         <v>11</v>
       </c>
-      <c r="H6" s="4" t="n">
+      <c r="H6" s="8">
         <v>500</v>
       </c>
-      <c r="I6" s="4" t="n">
+      <c r="I6" s="8">
         <v>2</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -909,14 +904,23 @@
       <c r="L6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="2" t="n">
+      <c r="M6" s="2">
         <v>20</v>
       </c>
-      <c r="N6" s="2" t="n">
+      <c r="N6" s="2">
         <v>48.8</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="7" s="8" spans="1:14">
+    <row r="7" spans="1:14" ht="15" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
       <c r="J7" s="2" t="s">
         <v>31</v>
       </c>
@@ -926,18 +930,27 @@
       <c r="L7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="2" t="n">
+      <c r="M7" s="2">
         <v>21</v>
       </c>
-      <c r="N7" s="2" t="n">
+      <c r="N7" s="2">
         <v>52.3</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="8" s="8" spans="1:14">
-      <c r="J8" s="6" t="s">
+    <row r="8" spans="1:14" ht="15" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="4" t="s">
         <v>29</v>
       </c>
       <c r="L8" s="2" t="s">
@@ -946,66 +959,62 @@
       <c r="M8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="2" t="n">
+      <c r="N8" s="2">
         <v>46.2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="I6:I8"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="D6:D8"/>
     <mergeCell ref="E6:E8"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="I6:I8"/>
   </mergeCells>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AMJ8"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D13" activeCellId="0" pane="topLeft" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="8" width="8.5748987854251"/>
-    <col customWidth="1" max="2" min="2" style="8" width="17.4251012145749"/>
-    <col customWidth="1" max="3" min="3" style="8" width="28.2874493927125"/>
-    <col customWidth="1" max="5" min="4" style="8" width="30.2874493927125"/>
-    <col customWidth="1" max="1025" min="6" style="8" width="8.5748987854251"/>
+    <col min="1" max="1" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="1024" width="8.5703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="8" spans="1:5">
-      <c r="A1" s="1" t="n"/>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="5"/>
+      <c r="B1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="10" t="n">
+      <c r="A2" s="7">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -1022,7 +1031,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="10" t="n">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -1039,7 +1048,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="10" t="n">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -1056,7 +1065,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="10" t="n">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -1073,7 +1082,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="10" t="n">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -1090,7 +1099,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="10" t="n">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -1107,7 +1116,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="10" t="n">
+      <c r="A8" s="7">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -1124,34 +1133,29 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AMK1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G10" activeCellId="0" pane="topLeft" sqref="G10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="8" width="8.5748987854251"/>
-    <col customWidth="1" max="2" min="2" style="8" width="13.7125506072874"/>
-    <col customWidth="1" max="3" min="3" style="8" width="10.5708502024292"/>
-    <col customWidth="1" max="1025" min="4" style="8" width="8.5748987854251"/>
+    <col min="1" max="1" width="8.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="6" customWidth="1"/>
+    <col min="4" max="1025" width="8.5703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="8" spans="1:3">
-      <c r="A1" s="1" t="n"/>
+    <row r="1" spans="1:3" ht="15" customHeight="1">
+      <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
@@ -1160,8 +1164,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>